<commit_message>
Added location to tables
</commit_message>
<xml_diff>
--- a/g2-04-he/helist.xlsx
+++ b/g2-04-he/helist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vanessakomar/Documents/Graz/2nd Semester/HCI/HCI/he/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M4ste\OneDrive\Desktop\HCI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CC65B5-2795-754E-BBEA-86DF196338A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003EA061-D52B-4978-83B0-D37F0DB7C17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1520" windowWidth="38400" windowHeight="21100" tabRatio="281" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="281" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problems" sheetId="4" r:id="rId1"/>
@@ -313,7 +313,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="249">
   <si>
     <t>No.</t>
   </si>
@@ -976,6 +976,141 @@
   </si>
   <si>
     <t>The site has information regarding the mobile app that the pharmacy has, however part of the information presented is a QR code which the user would not be able to scan as they are currently on the mobile site. This makes this information unnecessary.</t>
+  </si>
+  <si>
+    <t>n03-ru-neg06-navbar.mp4</t>
+  </si>
+  <si>
+    <t>n04-ks-neg07-fixed-place-for-buttons.mp4</t>
+  </si>
+  <si>
+    <t>n01-ru-neg05-site.mp4, n01-md-neg09-not-existing-sites.mp4</t>
+  </si>
+  <si>
+    <t>n05-ru-neg10-slide.mp4, n05-vk-neg08-text-inconsistencies.mp4</t>
+  </si>
+  <si>
+    <t>n02-vk-neg07-wishlist-nav.mp4</t>
+  </si>
+  <si>
+    <t>n06-md-neg04-list-of-products.mp4</t>
+  </si>
+  <si>
+    <t>n07-md-neg03-product-without-picture.mp4</t>
+  </si>
+  <si>
+    <t>n08-md-neg05-misleading-icons.mp4</t>
+  </si>
+  <si>
+    <t>n09-md-neg06-multiple-information-display.mp4</t>
+  </si>
+  <si>
+    <t>n10-ru-neg08-drop.mp4</t>
+  </si>
+  <si>
+    <t>n11-ks-neg10-opening-links.mp4</t>
+  </si>
+  <si>
+    <t>n12-vk-neg09-form-number.mp4</t>
+  </si>
+  <si>
+    <t>n13-vk-neg12-login-at-top.mp4</t>
+  </si>
+  <si>
+    <t>n14-vk-neg14-app-qrcode.mp4</t>
+  </si>
+  <si>
+    <t>n16-ru-neg01-pictures.mp4, n16-ru-neg02-map.mp4</t>
+  </si>
+  <si>
+    <t>n15-md-neg08-inconsistent-information.mp4</t>
+  </si>
+  <si>
+    <t>n17-ks-neg12-cut-off-screen.mp4</t>
+  </si>
+  <si>
+    <t>n18-ru-neg09-scroll.mp4</t>
+  </si>
+  <si>
+    <t>n20-ks-neg08-design-of-product-descriptions.mp4</t>
+  </si>
+  <si>
+    <t>n19-vk-neg10-logo-placement.mp4</t>
+  </si>
+  <si>
+    <t>n21-ks-neg09-extra-side-for-news.mp4</t>
+  </si>
+  <si>
+    <t>n22-ks-neg11-placed-links-disorderly.mp4</t>
+  </si>
+  <si>
+    <t>n23-vk-neg02-not-clickable.mp4</t>
+  </si>
+  <si>
+    <t>n24-md-neg02-picture-information.mp4</t>
+  </si>
+  <si>
+    <t>n25-md-neg11-no-indicator-similar-products.mp4</t>
+  </si>
+  <si>
+    <t>n26-ks-neg01-cookies-buttons-are-different.mp4</t>
+  </si>
+  <si>
+    <t>n27-ks-neg13-show-more-products.mp4</t>
+  </si>
+  <si>
+    <t>n28-vk-neg03-unnec-info.mp4</t>
+  </si>
+  <si>
+    <t>n29-md-neg01-shaking-pictures.mp4</t>
+  </si>
+  <si>
+    <t>n30-ks-neg03-unnecessary-links.mp4</t>
+  </si>
+  <si>
+    <t>n31-md-neg07-automatic-call.mp4</t>
+  </si>
+  <si>
+    <t>n32-ru-neg03-header.mp4</t>
+  </si>
+  <si>
+    <t>n33-ks-neg02-unpleasant-text-on-picture.mp4</t>
+  </si>
+  <si>
+    <t>n34-md-neg10-hard-navigation.mp4</t>
+  </si>
+  <si>
+    <t>p01-ks-pos02-available-product.mp4</t>
+  </si>
+  <si>
+    <t>p02-ks-pos03-fixed-bar.mp4</t>
+  </si>
+  <si>
+    <t>p03-md-pos02-alternatives-to-pharmacy.mp4</t>
+  </si>
+  <si>
+    <t>p04-ru-pos02-news.mp4</t>
+  </si>
+  <si>
+    <t>p05-md-pos03-appointment-formular.mp4</t>
+  </si>
+  <si>
+    <t>p06-ru-pos01-top.mp4</t>
+  </si>
+  <si>
+    <t>p07-ks-pos01-different-categories.mp4</t>
+  </si>
+  <si>
+    <t>p08-vk-pos02-breadcrumbs.mp4</t>
+  </si>
+  <si>
+    <t>p09-md-pos01-inviting-design</t>
+  </si>
+  <si>
+    <t>p10-vk-pos03-frage-form.mp4</t>
+  </si>
+  <si>
+    <t>p11-vk-pos01-form-field.mp4</t>
   </si>
 </sst>
 </file>
@@ -1033,12 +1168,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -1224,9 +1365,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1271,11 +1409,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{8EDDD985-0318-7F42-A08E-B5CF00DB257A}"/>
     <cellStyle name="Normal 3" xfId="2" xr:uid="{E00A8F0D-1E25-0A44-BDB6-5C6BB6D7932E}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1291,7 +1432,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1613,44 +1754,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F74010B2-EEEB-7C4E-9CAD-8D54C9129191}">
   <dimension ref="A1:V38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" style="11" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" style="11" customWidth="1"/>
-    <col min="5" max="5" width="27.1640625" style="11" customWidth="1"/>
-    <col min="6" max="6" width="15.33203125" style="11" customWidth="1"/>
-    <col min="7" max="7" width="17.5" style="11" customWidth="1"/>
-    <col min="8" max="8" width="27.6640625" style="11" customWidth="1"/>
-    <col min="9" max="9" width="3.83203125" style="11" customWidth="1"/>
-    <col min="10" max="10" width="3.1640625" style="11" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" style="11" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" style="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="11" customWidth="1"/>
+    <col min="8" max="8" width="27.7109375" style="11" customWidth="1"/>
+    <col min="9" max="9" width="3.85546875" style="11" customWidth="1"/>
+    <col min="10" max="10" width="3.140625" style="11" customWidth="1"/>
     <col min="11" max="11" width="3" style="11" customWidth="1"/>
-    <col min="12" max="12" width="2.83203125" style="11" customWidth="1"/>
-    <col min="13" max="13" width="3.33203125" style="11" customWidth="1"/>
+    <col min="12" max="12" width="2.85546875" style="11" customWidth="1"/>
+    <col min="13" max="13" width="3.28515625" style="11" customWidth="1"/>
     <col min="14" max="14" width="4" style="11" customWidth="1"/>
-    <col min="15" max="16" width="3.33203125" style="11" customWidth="1"/>
-    <col min="17" max="17" width="5.83203125" style="11" customWidth="1"/>
-    <col min="18" max="34" width="8.83203125" style="11" customWidth="1"/>
-    <col min="35" max="16384" width="8.83203125" style="11"/>
+    <col min="15" max="16" width="3.28515625" style="11" customWidth="1"/>
+    <col min="17" max="17" width="5.85546875" style="11" customWidth="1"/>
+    <col min="18" max="34" width="8.85546875" style="11" customWidth="1"/>
+    <col min="35" max="16384" width="8.85546875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="31.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:22" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="32" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="34" t="s">
+    <row r="2" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="33" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:22" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I3" s="20" t="s">
         <v>2</v>
       </c>
@@ -1660,11 +1801,11 @@
       </c>
       <c r="Q3" s="29"/>
     </row>
-    <row r="4" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:22" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="19" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="19" t="s">
@@ -1713,8 +1854,8 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="70" x14ac:dyDescent="0.15">
-      <c r="A5" s="32">
+    <row r="5" spans="1:22" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="31">
         <v>1</v>
       </c>
       <c r="B5" s="12" t="s">
@@ -1723,7 +1864,9 @@
       <c r="C5" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="D5" s="12"/>
+      <c r="D5" s="12" t="s">
+        <v>206</v>
+      </c>
       <c r="E5" s="12" t="s">
         <v>170</v>
       </c>
@@ -1740,20 +1883,20 @@
         <v>4</v>
       </c>
       <c r="L5" s="26"/>
-      <c r="M5" s="41">
-        <v>4</v>
-      </c>
-      <c r="N5" s="40">
-        <v>4</v>
-      </c>
-      <c r="O5" s="40">
-        <v>3</v>
-      </c>
-      <c r="P5" s="40">
+      <c r="M5" s="40">
+        <v>4</v>
+      </c>
+      <c r="N5" s="39">
+        <v>4</v>
+      </c>
+      <c r="O5" s="39">
+        <v>3</v>
+      </c>
+      <c r="P5" s="39">
         <v>3</v>
       </c>
       <c r="Q5" s="27">
-        <f>AVERAGE(M5:P5)</f>
+        <f t="shared" ref="Q5:Q38" si="0">AVERAGE(M5:P5)</f>
         <v>3.5</v>
       </c>
       <c r="R5" s="12"/>
@@ -1762,8 +1905,8 @@
       <c r="U5" s="12"/>
       <c r="V5" s="12"/>
     </row>
-    <row r="6" spans="1:22" s="14" customFormat="1" ht="70" x14ac:dyDescent="0.2">
-      <c r="A6" s="32">
+    <row r="6" spans="1:22" s="14" customFormat="1" ht="76.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="31">
         <v>2</v>
       </c>
       <c r="B6" s="12" t="s">
@@ -1772,7 +1915,9 @@
       <c r="C6" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="D6" s="12"/>
+      <c r="D6" s="12" t="s">
+        <v>208</v>
+      </c>
       <c r="E6" s="12" t="s">
         <v>76</v>
       </c>
@@ -1793,25 +1938,25 @@
       <c r="L6" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="41">
-        <v>3</v>
-      </c>
-      <c r="N6" s="40">
-        <v>2</v>
-      </c>
-      <c r="O6" s="40">
-        <v>4</v>
-      </c>
-      <c r="P6" s="40">
+      <c r="M6" s="40">
+        <v>3</v>
+      </c>
+      <c r="N6" s="39">
+        <v>2</v>
+      </c>
+      <c r="O6" s="39">
+        <v>4</v>
+      </c>
+      <c r="P6" s="39">
         <v>4</v>
       </c>
       <c r="Q6" s="27">
-        <f>AVERAGE(M6:P6)</f>
+        <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="113" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="32">
+    <row r="7" spans="1:22" ht="113.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="31">
         <v>3</v>
       </c>
       <c r="B7" s="12" t="s">
@@ -1820,7 +1965,9 @@
       <c r="C7" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="D7" s="12"/>
+      <c r="D7" s="12" t="s">
+        <v>204</v>
+      </c>
       <c r="E7" s="12" t="s">
         <v>87</v>
       </c>
@@ -1839,25 +1986,25 @@
       <c r="L7" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="41">
-        <v>2</v>
-      </c>
-      <c r="N7" s="40">
-        <v>3</v>
-      </c>
-      <c r="O7" s="40">
-        <v>3</v>
-      </c>
-      <c r="P7" s="40">
+      <c r="M7" s="40">
+        <v>2</v>
+      </c>
+      <c r="N7" s="39">
+        <v>3</v>
+      </c>
+      <c r="O7" s="39">
+        <v>3</v>
+      </c>
+      <c r="P7" s="39">
         <v>4</v>
       </c>
       <c r="Q7" s="27">
-        <f>AVERAGE(M7:P7)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" ht="154" x14ac:dyDescent="0.15">
-      <c r="A8" s="32">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="A8" s="31">
         <v>4</v>
       </c>
       <c r="B8" s="12" t="s">
@@ -1866,7 +2013,9 @@
       <c r="C8" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="D8" s="12"/>
+      <c r="D8" s="12" t="s">
+        <v>205</v>
+      </c>
       <c r="E8" s="12" t="s">
         <v>91</v>
       </c>
@@ -1887,25 +2036,25 @@
       <c r="L8" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="M8" s="41">
-        <v>3</v>
-      </c>
-      <c r="N8" s="40">
-        <v>3</v>
-      </c>
-      <c r="O8" s="40">
-        <v>2</v>
-      </c>
-      <c r="P8" s="40">
+      <c r="M8" s="40">
+        <v>3</v>
+      </c>
+      <c r="N8" s="39">
+        <v>3</v>
+      </c>
+      <c r="O8" s="39">
+        <v>2</v>
+      </c>
+      <c r="P8" s="39">
         <v>3</v>
       </c>
       <c r="Q8" s="27">
-        <f>AVERAGE(M8:P8)</f>
+        <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="154" x14ac:dyDescent="0.15">
-      <c r="A9" s="32">
+    <row r="9" spans="1:22" ht="140.25" x14ac:dyDescent="0.2">
+      <c r="A9" s="31">
         <v>5</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -1914,7 +2063,9 @@
       <c r="C9" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="D9" s="12"/>
+      <c r="D9" s="12" t="s">
+        <v>207</v>
+      </c>
       <c r="E9" s="12" t="s">
         <v>117</v>
       </c>
@@ -1931,25 +2082,25 @@
         <v>4</v>
       </c>
       <c r="L9" s="26"/>
-      <c r="M9" s="41">
-        <v>2</v>
-      </c>
-      <c r="N9" s="40">
-        <v>3</v>
-      </c>
-      <c r="O9" s="40">
-        <v>3</v>
-      </c>
-      <c r="P9" s="40">
+      <c r="M9" s="40">
+        <v>2</v>
+      </c>
+      <c r="N9" s="39">
+        <v>3</v>
+      </c>
+      <c r="O9" s="39">
+        <v>3</v>
+      </c>
+      <c r="P9" s="39">
         <v>3</v>
       </c>
       <c r="Q9" s="27">
-        <f>AVERAGE(M9:P9)</f>
+        <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="84" x14ac:dyDescent="0.15">
-      <c r="A10" s="32">
+    <row r="10" spans="1:22" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A10" s="31">
         <v>6</v>
       </c>
       <c r="B10" s="12" t="s">
@@ -1958,7 +2109,9 @@
       <c r="C10" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="D10" s="12"/>
+      <c r="D10" s="12" t="s">
+        <v>209</v>
+      </c>
       <c r="E10" s="12" t="s">
         <v>159</v>
       </c>
@@ -1977,25 +2130,25 @@
       <c r="L10" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="M10" s="41">
-        <v>2</v>
-      </c>
-      <c r="N10" s="40">
-        <v>3</v>
-      </c>
-      <c r="O10" s="40">
-        <v>3</v>
-      </c>
-      <c r="P10" s="40">
+      <c r="M10" s="40">
+        <v>2</v>
+      </c>
+      <c r="N10" s="39">
+        <v>3</v>
+      </c>
+      <c r="O10" s="39">
+        <v>3</v>
+      </c>
+      <c r="P10" s="39">
         <v>2</v>
       </c>
       <c r="Q10" s="27">
-        <f>AVERAGE(M10:P10)</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="56" x14ac:dyDescent="0.15">
-      <c r="A11" s="32">
+    <row r="11" spans="1:22" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A11" s="31">
         <v>7</v>
       </c>
       <c r="B11" s="12" t="s">
@@ -2004,7 +2157,9 @@
       <c r="C11" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="D11" s="12"/>
+      <c r="D11" s="12" t="s">
+        <v>210</v>
+      </c>
       <c r="E11" s="12" t="s">
         <v>157</v>
       </c>
@@ -2021,25 +2176,25 @@
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="26"/>
-      <c r="M11" s="41">
-        <v>2</v>
-      </c>
-      <c r="N11" s="32">
-        <v>3</v>
-      </c>
-      <c r="O11" s="40">
-        <v>3</v>
-      </c>
-      <c r="P11" s="32">
+      <c r="M11" s="40">
+        <v>2</v>
+      </c>
+      <c r="N11" s="31">
+        <v>3</v>
+      </c>
+      <c r="O11" s="39">
+        <v>3</v>
+      </c>
+      <c r="P11" s="31">
         <v>2</v>
       </c>
       <c r="Q11" s="27">
-        <f>AVERAGE(M11:P11)</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="70" x14ac:dyDescent="0.15">
-      <c r="A12" s="32">
+    <row r="12" spans="1:22" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="31">
         <v>8</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -2048,7 +2203,9 @@
       <c r="C12" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="D12" s="12"/>
+      <c r="D12" s="12" t="s">
+        <v>211</v>
+      </c>
       <c r="E12" s="12" t="s">
         <v>160</v>
       </c>
@@ -2064,25 +2221,25 @@
         <v>4</v>
       </c>
       <c r="L12" s="13"/>
-      <c r="M12" s="41">
-        <v>2</v>
-      </c>
-      <c r="N12" s="40">
-        <v>2</v>
-      </c>
-      <c r="O12" s="40">
-        <v>2</v>
-      </c>
-      <c r="P12" s="40">
+      <c r="M12" s="40">
+        <v>2</v>
+      </c>
+      <c r="N12" s="39">
+        <v>2</v>
+      </c>
+      <c r="O12" s="39">
+        <v>2</v>
+      </c>
+      <c r="P12" s="39">
         <v>3</v>
       </c>
       <c r="Q12" s="27">
-        <f>AVERAGE(M12:P12)</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="32">
+    <row r="13" spans="1:22" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="31">
         <v>9</v>
       </c>
       <c r="B13" s="12" t="s">
@@ -2091,7 +2248,9 @@
       <c r="C13" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="D13" s="12"/>
+      <c r="D13" s="12" t="s">
+        <v>212</v>
+      </c>
       <c r="E13" s="12" t="s">
         <v>163</v>
       </c>
@@ -2107,26 +2266,26 @@
         <v>4</v>
       </c>
       <c r="L13" s="13"/>
-      <c r="M13" s="41">
-        <v>2</v>
-      </c>
-      <c r="N13" s="40">
-        <v>2</v>
-      </c>
-      <c r="O13" s="40">
-        <v>3</v>
-      </c>
-      <c r="P13" s="40">
+      <c r="M13" s="40">
+        <v>2</v>
+      </c>
+      <c r="N13" s="39">
+        <v>2</v>
+      </c>
+      <c r="O13" s="39">
+        <v>3</v>
+      </c>
+      <c r="P13" s="39">
         <v>2</v>
       </c>
       <c r="Q13" s="27">
-        <f>AVERAGE(M13:P13)</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
       <c r="R13" s="12"/>
     </row>
-    <row r="14" spans="1:22" ht="60" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="32">
+    <row r="14" spans="1:22" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="31">
         <v>10</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -2135,7 +2294,9 @@
       <c r="C14" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="D14" s="12"/>
+      <c r="D14" s="12" t="s">
+        <v>213</v>
+      </c>
       <c r="E14" s="12" t="s">
         <v>96</v>
       </c>
@@ -2154,26 +2315,26 @@
         <v>4</v>
       </c>
       <c r="L14" s="26"/>
-      <c r="M14" s="41">
-        <v>2</v>
-      </c>
-      <c r="N14" s="40">
-        <v>1</v>
-      </c>
-      <c r="O14" s="40">
-        <v>3</v>
-      </c>
-      <c r="P14" s="40">
+      <c r="M14" s="40">
+        <v>2</v>
+      </c>
+      <c r="N14" s="39">
+        <v>1</v>
+      </c>
+      <c r="O14" s="39">
+        <v>3</v>
+      </c>
+      <c r="P14" s="39">
         <v>2</v>
       </c>
       <c r="Q14" s="27">
-        <f>AVERAGE(M14:P14)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R14" s="12"/>
     </row>
-    <row r="15" spans="1:22" ht="56" x14ac:dyDescent="0.15">
-      <c r="A15" s="32">
+    <row r="15" spans="1:22" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="31">
         <v>11</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -2182,7 +2343,9 @@
       <c r="C15" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="12"/>
+      <c r="D15" s="12" t="s">
+        <v>214</v>
+      </c>
       <c r="E15" s="12" t="s">
         <v>51</v>
       </c>
@@ -2199,26 +2362,26 @@
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="26"/>
-      <c r="M15" s="41">
-        <v>3</v>
-      </c>
-      <c r="N15" s="40">
-        <v>2</v>
-      </c>
-      <c r="O15" s="40">
-        <v>1</v>
-      </c>
-      <c r="P15" s="40">
+      <c r="M15" s="40">
+        <v>3</v>
+      </c>
+      <c r="N15" s="39">
+        <v>2</v>
+      </c>
+      <c r="O15" s="39">
+        <v>1</v>
+      </c>
+      <c r="P15" s="39">
         <v>2</v>
       </c>
       <c r="Q15" s="27">
-        <f>AVERAGE(M15:P15)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="R15" s="12"/>
     </row>
-    <row r="16" spans="1:22" ht="70" x14ac:dyDescent="0.15">
-      <c r="A16" s="32">
+    <row r="16" spans="1:22" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A16" s="31">
         <v>12</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -2227,7 +2390,9 @@
       <c r="C16" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="12"/>
+      <c r="D16" s="12" t="s">
+        <v>215</v>
+      </c>
       <c r="E16" s="12" t="s">
         <v>64</v>
       </c>
@@ -2244,25 +2409,25 @@
       <c r="L16" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="M16" s="41">
-        <v>2</v>
-      </c>
-      <c r="N16" s="32">
-        <v>1</v>
-      </c>
-      <c r="O16" s="40">
-        <v>3</v>
-      </c>
-      <c r="P16" s="40">
+      <c r="M16" s="40">
+        <v>2</v>
+      </c>
+      <c r="N16" s="31">
+        <v>1</v>
+      </c>
+      <c r="O16" s="39">
+        <v>3</v>
+      </c>
+      <c r="P16" s="39">
         <v>2</v>
       </c>
       <c r="Q16" s="27">
-        <f>AVERAGE(M16:P16)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" ht="56" x14ac:dyDescent="0.15">
-      <c r="A17" s="32">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="A17" s="31">
         <v>13</v>
       </c>
       <c r="B17" s="12" t="s">
@@ -2271,7 +2436,9 @@
       <c r="C17" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="D17" s="12"/>
+      <c r="D17" s="12" t="s">
+        <v>216</v>
+      </c>
       <c r="E17" s="12" t="s">
         <v>65</v>
       </c>
@@ -2290,25 +2457,25 @@
       <c r="L17" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="M17" s="41">
-        <v>2</v>
-      </c>
-      <c r="N17" s="40">
-        <v>2</v>
-      </c>
-      <c r="O17" s="40">
-        <v>2</v>
-      </c>
-      <c r="P17" s="40">
+      <c r="M17" s="40">
+        <v>2</v>
+      </c>
+      <c r="N17" s="39">
+        <v>2</v>
+      </c>
+      <c r="O17" s="39">
+        <v>2</v>
+      </c>
+      <c r="P17" s="39">
         <v>2</v>
       </c>
       <c r="Q17" s="27">
-        <f>AVERAGE(M17:P17)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" ht="84" x14ac:dyDescent="0.15">
-      <c r="A18" s="32">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A18" s="31">
         <v>14</v>
       </c>
       <c r="B18" s="12" t="s">
@@ -2317,7 +2484,9 @@
       <c r="C18" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="D18" s="12"/>
+      <c r="D18" s="12" t="s">
+        <v>217</v>
+      </c>
       <c r="E18" s="12" t="s">
         <v>66</v>
       </c>
@@ -2336,25 +2505,25 @@
       <c r="L18" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="M18" s="41">
-        <v>1</v>
-      </c>
-      <c r="N18" s="40">
-        <v>3</v>
-      </c>
-      <c r="O18" s="40">
-        <v>2</v>
-      </c>
-      <c r="P18" s="40">
+      <c r="M18" s="40">
+        <v>1</v>
+      </c>
+      <c r="N18" s="39">
+        <v>3</v>
+      </c>
+      <c r="O18" s="39">
+        <v>2</v>
+      </c>
+      <c r="P18" s="39">
         <v>2</v>
       </c>
       <c r="Q18" s="27">
-        <f>AVERAGE(M18:P18)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="70" x14ac:dyDescent="0.15">
-      <c r="A19" s="32">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A19" s="31">
         <v>15</v>
       </c>
       <c r="B19" s="12" t="s">
@@ -2363,7 +2532,9 @@
       <c r="C19" s="12" t="s">
         <v>195</v>
       </c>
-      <c r="D19" s="12"/>
+      <c r="D19" s="12" t="s">
+        <v>219</v>
+      </c>
       <c r="E19" s="12" t="s">
         <v>168</v>
       </c>
@@ -2379,25 +2550,25 @@
         <v>4</v>
       </c>
       <c r="L19" s="13"/>
-      <c r="M19" s="41">
-        <v>2</v>
-      </c>
-      <c r="N19" s="40">
-        <v>2</v>
-      </c>
-      <c r="O19" s="40">
-        <v>2</v>
-      </c>
-      <c r="P19" s="40">
+      <c r="M19" s="40">
+        <v>2</v>
+      </c>
+      <c r="N19" s="39">
+        <v>2</v>
+      </c>
+      <c r="O19" s="39">
+        <v>2</v>
+      </c>
+      <c r="P19" s="39">
         <v>2</v>
       </c>
       <c r="Q19" s="27">
-        <f>AVERAGE(M19:P19)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" ht="56" x14ac:dyDescent="0.15">
-      <c r="A20" s="32">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+      <c r="A20" s="31">
         <v>16</v>
       </c>
       <c r="B20" s="12" t="s">
@@ -2406,7 +2577,9 @@
       <c r="C20" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="D20" s="12"/>
+      <c r="D20" s="12" t="s">
+        <v>218</v>
+      </c>
       <c r="E20" s="12" t="s">
         <v>94</v>
       </c>
@@ -2423,25 +2596,25 @@
         <v>4</v>
       </c>
       <c r="L20" s="26"/>
-      <c r="M20" s="41">
-        <v>2</v>
-      </c>
-      <c r="N20" s="40">
-        <v>2</v>
-      </c>
-      <c r="O20" s="40">
-        <v>1</v>
-      </c>
-      <c r="P20" s="40">
+      <c r="M20" s="40">
+        <v>2</v>
+      </c>
+      <c r="N20" s="39">
+        <v>2</v>
+      </c>
+      <c r="O20" s="39">
+        <v>1</v>
+      </c>
+      <c r="P20" s="39">
         <v>2</v>
       </c>
       <c r="Q20" s="27">
-        <f>AVERAGE(M20:P20)</f>
+        <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="21" spans="1:18" ht="70" x14ac:dyDescent="0.15">
-      <c r="A21" s="32">
+    <row r="21" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A21" s="31">
         <v>17</v>
       </c>
       <c r="B21" s="12" t="s">
@@ -2450,7 +2623,9 @@
       <c r="C21" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="12"/>
+      <c r="D21" s="12" t="s">
+        <v>220</v>
+      </c>
       <c r="E21" s="12" t="s">
         <v>84</v>
       </c>
@@ -2467,25 +2642,25 @@
         <v>4</v>
       </c>
       <c r="L21" s="26"/>
-      <c r="M21" s="41">
-        <v>4</v>
-      </c>
-      <c r="N21" s="40">
-        <v>1</v>
-      </c>
-      <c r="O21" s="40">
-        <v>1</v>
-      </c>
-      <c r="P21" s="40">
+      <c r="M21" s="40">
+        <v>4</v>
+      </c>
+      <c r="N21" s="39">
+        <v>1</v>
+      </c>
+      <c r="O21" s="39">
+        <v>1</v>
+      </c>
+      <c r="P21" s="39">
         <v>1</v>
       </c>
       <c r="Q21" s="27">
-        <f>AVERAGE(M21:P21)</f>
+        <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="22" spans="1:18" ht="42" x14ac:dyDescent="0.15">
-      <c r="A22" s="32">
+    <row r="22" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="A22" s="31">
         <v>18</v>
       </c>
       <c r="B22" s="12" t="s">
@@ -2494,7 +2669,9 @@
       <c r="C22" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D22" s="12"/>
+      <c r="D22" s="12" t="s">
+        <v>221</v>
+      </c>
       <c r="E22" s="12" t="s">
         <v>30</v>
       </c>
@@ -2513,25 +2690,25 @@
         <v>4</v>
       </c>
       <c r="L22" s="26"/>
-      <c r="M22" s="41">
-        <v>2</v>
-      </c>
-      <c r="N22" s="40">
-        <v>2</v>
-      </c>
-      <c r="O22" s="40">
-        <v>2</v>
-      </c>
-      <c r="P22" s="40">
+      <c r="M22" s="40">
+        <v>2</v>
+      </c>
+      <c r="N22" s="39">
+        <v>2</v>
+      </c>
+      <c r="O22" s="39">
+        <v>2</v>
+      </c>
+      <c r="P22" s="39">
         <v>1</v>
       </c>
       <c r="Q22" s="27">
-        <f>AVERAGE(M22:P22)</f>
+        <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="84" x14ac:dyDescent="0.15">
-      <c r="A23" s="32">
+    <row r="23" spans="1:18" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="31">
         <v>19</v>
       </c>
       <c r="B23" s="12" t="s">
@@ -2540,7 +2717,9 @@
       <c r="C23" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="D23" s="12"/>
+      <c r="D23" s="12" t="s">
+        <v>223</v>
+      </c>
       <c r="E23" s="12" t="s">
         <v>81</v>
       </c>
@@ -2559,25 +2738,25 @@
       <c r="L23" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="M23" s="46">
-        <v>3</v>
-      </c>
-      <c r="N23" s="40">
-        <v>1</v>
-      </c>
-      <c r="O23" s="40">
-        <v>2</v>
-      </c>
-      <c r="P23" s="40">
+      <c r="M23" s="45">
+        <v>3</v>
+      </c>
+      <c r="N23" s="39">
+        <v>1</v>
+      </c>
+      <c r="O23" s="39">
+        <v>2</v>
+      </c>
+      <c r="P23" s="39">
         <v>1</v>
       </c>
       <c r="Q23" s="27">
-        <f>AVERAGE(M23:P23)</f>
+        <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="143" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="32">
+    <row r="24" spans="1:18" ht="143.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="31">
         <v>20</v>
       </c>
       <c r="B24" s="12" t="s">
@@ -2586,7 +2765,9 @@
       <c r="C24" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="D24" s="12"/>
+      <c r="D24" s="12" t="s">
+        <v>222</v>
+      </c>
       <c r="E24" s="12" t="s">
         <v>47</v>
       </c>
@@ -2603,25 +2784,25 @@
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="26"/>
-      <c r="M24" s="41">
-        <v>2</v>
-      </c>
-      <c r="N24" s="40">
-        <v>2</v>
-      </c>
-      <c r="O24" s="40">
-        <v>2</v>
-      </c>
-      <c r="P24" s="40">
+      <c r="M24" s="40">
+        <v>2</v>
+      </c>
+      <c r="N24" s="39">
+        <v>2</v>
+      </c>
+      <c r="O24" s="39">
+        <v>2</v>
+      </c>
+      <c r="P24" s="39">
         <v>1</v>
       </c>
       <c r="Q24" s="27">
-        <f>AVERAGE(M24:P24)</f>
+        <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="25" spans="1:18" ht="70" x14ac:dyDescent="0.15">
-      <c r="A25" s="32">
+    <row r="25" spans="1:18" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A25" s="31">
         <v>21</v>
       </c>
       <c r="B25" s="12" t="s">
@@ -2630,7 +2811,9 @@
       <c r="C25" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="D25" s="12"/>
+      <c r="D25" s="12" t="s">
+        <v>224</v>
+      </c>
       <c r="E25" s="12" t="s">
         <v>48</v>
       </c>
@@ -2647,25 +2830,25 @@
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="26"/>
-      <c r="M25" s="41">
-        <v>2</v>
-      </c>
-      <c r="N25" s="40">
-        <v>2</v>
-      </c>
-      <c r="O25" s="40">
-        <v>2</v>
-      </c>
-      <c r="P25" s="40">
+      <c r="M25" s="40">
+        <v>2</v>
+      </c>
+      <c r="N25" s="39">
+        <v>2</v>
+      </c>
+      <c r="O25" s="39">
+        <v>2</v>
+      </c>
+      <c r="P25" s="39">
         <v>1</v>
       </c>
       <c r="Q25" s="27">
-        <f>AVERAGE(M25:P25)</f>
+        <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="26" spans="1:18" ht="42" x14ac:dyDescent="0.15">
-      <c r="A26" s="32">
+    <row r="26" spans="1:18" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A26" s="31">
         <v>22</v>
       </c>
       <c r="B26" s="12" t="s">
@@ -2674,7 +2857,9 @@
       <c r="C26" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D26" s="12"/>
+      <c r="D26" s="12" t="s">
+        <v>225</v>
+      </c>
       <c r="E26" s="12" t="s">
         <v>55</v>
       </c>
@@ -2691,25 +2876,25 @@
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
       <c r="L26" s="26"/>
-      <c r="M26" s="41">
-        <v>2</v>
-      </c>
-      <c r="N26" s="40">
-        <v>1</v>
-      </c>
-      <c r="O26" s="40">
-        <v>3</v>
-      </c>
-      <c r="P26" s="40">
+      <c r="M26" s="40">
+        <v>2</v>
+      </c>
+      <c r="N26" s="39">
+        <v>1</v>
+      </c>
+      <c r="O26" s="39">
+        <v>3</v>
+      </c>
+      <c r="P26" s="39">
         <v>1</v>
       </c>
       <c r="Q26" s="27">
-        <f>AVERAGE(M26:P26)</f>
+        <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="27" spans="1:18" ht="84" x14ac:dyDescent="0.15">
-      <c r="A27" s="32">
+    <row r="27" spans="1:18" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A27" s="31">
         <v>23</v>
       </c>
       <c r="B27" s="12" t="s">
@@ -2718,7 +2903,9 @@
       <c r="C27" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="D27" s="12"/>
+      <c r="D27" s="12" t="s">
+        <v>226</v>
+      </c>
       <c r="E27" s="12" t="s">
         <v>62</v>
       </c>
@@ -2735,25 +2922,25 @@
       <c r="L27" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="M27" s="41">
-        <v>2</v>
-      </c>
-      <c r="N27" s="40">
-        <v>2</v>
-      </c>
-      <c r="O27" s="40">
-        <v>1</v>
-      </c>
-      <c r="P27" s="40">
+      <c r="M27" s="40">
+        <v>2</v>
+      </c>
+      <c r="N27" s="39">
+        <v>2</v>
+      </c>
+      <c r="O27" s="39">
+        <v>1</v>
+      </c>
+      <c r="P27" s="39">
         <v>2</v>
       </c>
       <c r="Q27" s="27">
-        <f>AVERAGE(M27:P27)</f>
+        <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="56" x14ac:dyDescent="0.15">
-      <c r="A28" s="32">
+    <row r="28" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="31">
         <v>24</v>
       </c>
       <c r="B28" s="12" t="s">
@@ -2762,7 +2949,9 @@
       <c r="C28" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="D28" s="12"/>
+      <c r="D28" s="12" t="s">
+        <v>227</v>
+      </c>
       <c r="E28" s="12" t="s">
         <v>155</v>
       </c>
@@ -2779,25 +2968,25 @@
       </c>
       <c r="K28" s="12"/>
       <c r="L28" s="26"/>
-      <c r="M28" s="41">
-        <v>2</v>
-      </c>
-      <c r="N28" s="32">
-        <v>2</v>
-      </c>
-      <c r="O28" s="40">
-        <v>2</v>
-      </c>
-      <c r="P28" s="32">
+      <c r="M28" s="40">
+        <v>2</v>
+      </c>
+      <c r="N28" s="31">
+        <v>2</v>
+      </c>
+      <c r="O28" s="39">
+        <v>2</v>
+      </c>
+      <c r="P28" s="31">
         <v>1</v>
       </c>
       <c r="Q28" s="27">
-        <f>AVERAGE(M28:P28)</f>
+        <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="29" spans="1:18" ht="56" x14ac:dyDescent="0.15">
-      <c r="A29" s="32">
+    <row r="29" spans="1:18" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A29" s="31">
         <v>25</v>
       </c>
       <c r="B29" s="12" t="s">
@@ -2806,7 +2995,9 @@
       <c r="C29" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="D29" s="12"/>
+      <c r="D29" s="12" t="s">
+        <v>228</v>
+      </c>
       <c r="E29" s="12" t="s">
         <v>174</v>
       </c>
@@ -2822,25 +3013,25 @@
         <v>4</v>
       </c>
       <c r="L29" s="13"/>
-      <c r="M29" s="41">
-        <v>3</v>
-      </c>
-      <c r="N29" s="40">
-        <v>2</v>
-      </c>
-      <c r="O29" s="40">
-        <v>1</v>
-      </c>
-      <c r="P29" s="40">
+      <c r="M29" s="40">
+        <v>3</v>
+      </c>
+      <c r="N29" s="39">
+        <v>2</v>
+      </c>
+      <c r="O29" s="39">
+        <v>1</v>
+      </c>
+      <c r="P29" s="39">
         <v>1</v>
       </c>
       <c r="Q29" s="27">
-        <f>AVERAGE(M29:P29)</f>
+        <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="30" spans="1:18" ht="42" x14ac:dyDescent="0.15">
-      <c r="A30" s="32">
+    <row r="30" spans="1:18" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A30" s="31">
         <v>26</v>
       </c>
       <c r="B30" s="12" t="s">
@@ -2849,7 +3040,9 @@
       <c r="C30" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D30" s="12"/>
+      <c r="D30" s="12" t="s">
+        <v>229</v>
+      </c>
       <c r="E30" s="12" t="s">
         <v>35</v>
       </c>
@@ -2865,27 +3058,27 @@
       </c>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
-      <c r="L30" s="45"/>
-      <c r="M30" s="41">
-        <v>2</v>
-      </c>
-      <c r="N30" s="40">
-        <v>2</v>
-      </c>
-      <c r="O30" s="40">
-        <v>1</v>
-      </c>
-      <c r="P30" s="40">
+      <c r="L30" s="44"/>
+      <c r="M30" s="40">
+        <v>2</v>
+      </c>
+      <c r="N30" s="39">
+        <v>2</v>
+      </c>
+      <c r="O30" s="39">
+        <v>1</v>
+      </c>
+      <c r="P30" s="39">
         <v>1</v>
       </c>
       <c r="Q30" s="27">
-        <f>AVERAGE(M30:P30)</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="R30" s="25"/>
     </row>
-    <row r="31" spans="1:18" ht="42" x14ac:dyDescent="0.15">
-      <c r="A31" s="32">
+    <row r="31" spans="1:18" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A31" s="31">
         <v>27</v>
       </c>
       <c r="B31" s="12" t="s">
@@ -2894,7 +3087,9 @@
       <c r="C31" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="D31" s="12"/>
+      <c r="D31" s="12" t="s">
+        <v>230</v>
+      </c>
       <c r="E31" s="12" t="s">
         <v>56</v>
       </c>
@@ -2910,27 +3105,27 @@
       </c>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
-      <c r="L31" s="45"/>
-      <c r="M31" s="41">
-        <v>2</v>
-      </c>
-      <c r="N31" s="40">
-        <v>2</v>
-      </c>
-      <c r="O31" s="40">
-        <v>1</v>
-      </c>
-      <c r="P31" s="40">
+      <c r="L31" s="44"/>
+      <c r="M31" s="40">
+        <v>2</v>
+      </c>
+      <c r="N31" s="39">
+        <v>2</v>
+      </c>
+      <c r="O31" s="39">
+        <v>1</v>
+      </c>
+      <c r="P31" s="39">
         <v>1</v>
       </c>
       <c r="Q31" s="27">
-        <f>AVERAGE(M31:P31)</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="R31" s="25"/>
     </row>
-    <row r="32" spans="1:18" ht="70" x14ac:dyDescent="0.15">
-      <c r="A32" s="32">
+    <row r="32" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="31">
         <v>28</v>
       </c>
       <c r="B32" s="12" t="s">
@@ -2938,6 +3133,9 @@
       </c>
       <c r="C32" s="12" t="s">
         <v>151</v>
+      </c>
+      <c r="D32" s="12" t="s">
+        <v>231</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>63</v>
@@ -2954,29 +3152,29 @@
       <c r="I32" s="28"/>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
-      <c r="L32" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="M32" s="41">
-        <v>1</v>
-      </c>
-      <c r="N32" s="40">
-        <v>1</v>
-      </c>
-      <c r="O32" s="40">
-        <v>3</v>
-      </c>
-      <c r="P32" s="40">
+      <c r="L32" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="M32" s="40">
+        <v>1</v>
+      </c>
+      <c r="N32" s="39">
+        <v>1</v>
+      </c>
+      <c r="O32" s="39">
+        <v>3</v>
+      </c>
+      <c r="P32" s="39">
         <v>1</v>
       </c>
       <c r="Q32" s="27">
-        <f>AVERAGE(M32:P32)</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="R32" s="25"/>
     </row>
-    <row r="33" spans="1:18" ht="42" x14ac:dyDescent="0.15">
-      <c r="A33" s="32">
+    <row r="33" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A33" s="31">
         <v>29</v>
       </c>
       <c r="B33" s="12" t="s">
@@ -2985,7 +3183,9 @@
       <c r="C33" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="D33" s="12"/>
+      <c r="D33" s="12" t="s">
+        <v>232</v>
+      </c>
       <c r="E33" s="12" t="s">
         <v>153</v>
       </c>
@@ -3004,26 +3204,26 @@
       </c>
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
-      <c r="M33" s="41">
-        <v>1</v>
-      </c>
-      <c r="N33" s="32">
-        <v>1</v>
-      </c>
-      <c r="O33" s="40">
-        <v>3</v>
-      </c>
-      <c r="P33" s="32">
+      <c r="M33" s="40">
+        <v>1</v>
+      </c>
+      <c r="N33" s="31">
+        <v>1</v>
+      </c>
+      <c r="O33" s="39">
+        <v>3</v>
+      </c>
+      <c r="P33" s="31">
         <v>1</v>
       </c>
       <c r="Q33" s="27">
-        <f>AVERAGE(M33:P33)</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
       <c r="R33" s="25"/>
     </row>
-    <row r="34" spans="1:18" ht="42" x14ac:dyDescent="0.15">
-      <c r="A34" s="32">
+    <row r="34" spans="1:18" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A34" s="31">
         <v>30</v>
       </c>
       <c r="B34" s="12" t="s">
@@ -3032,7 +3232,9 @@
       <c r="C34" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D34" s="12"/>
+      <c r="D34" s="12" t="s">
+        <v>233</v>
+      </c>
       <c r="E34" s="12" t="s">
         <v>43</v>
       </c>
@@ -3048,27 +3250,27 @@
       </c>
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
-      <c r="L34" s="45"/>
-      <c r="M34" s="41">
-        <v>1</v>
-      </c>
-      <c r="N34" s="40">
-        <v>1</v>
-      </c>
-      <c r="O34" s="40">
-        <v>1</v>
-      </c>
-      <c r="P34" s="40">
+      <c r="L34" s="44"/>
+      <c r="M34" s="40">
+        <v>1</v>
+      </c>
+      <c r="N34" s="39">
+        <v>1</v>
+      </c>
+      <c r="O34" s="39">
+        <v>1</v>
+      </c>
+      <c r="P34" s="39">
         <v>2</v>
       </c>
       <c r="Q34" s="27">
-        <f>AVERAGE(M34:P34)</f>
+        <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
       <c r="R34" s="25"/>
     </row>
-    <row r="35" spans="1:18" ht="56" x14ac:dyDescent="0.15">
-      <c r="A35" s="32">
+    <row r="35" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A35" s="31">
         <v>31</v>
       </c>
       <c r="B35" s="12" t="s">
@@ -3077,7 +3279,9 @@
       <c r="C35" s="12" t="s">
         <v>165</v>
       </c>
-      <c r="D35" s="12"/>
+      <c r="D35" s="12" t="s">
+        <v>234</v>
+      </c>
       <c r="E35" s="12" t="s">
         <v>166</v>
       </c>
@@ -3092,26 +3296,26 @@
       <c r="J35" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M35" s="41">
-        <v>1</v>
-      </c>
-      <c r="N35" s="40">
-        <v>1</v>
-      </c>
-      <c r="O35" s="40">
-        <v>2</v>
-      </c>
-      <c r="P35" s="40">
+      <c r="M35" s="40">
+        <v>1</v>
+      </c>
+      <c r="N35" s="39">
+        <v>1</v>
+      </c>
+      <c r="O35" s="39">
+        <v>2</v>
+      </c>
+      <c r="P35" s="39">
         <v>1</v>
       </c>
       <c r="Q35" s="27">
-        <f>AVERAGE(M35:P35)</f>
+        <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
       <c r="R35" s="25"/>
     </row>
-    <row r="36" spans="1:18" ht="42" x14ac:dyDescent="0.15">
-      <c r="A36" s="32">
+    <row r="36" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="A36" s="31">
         <v>32</v>
       </c>
       <c r="B36" s="12" t="s">
@@ -3120,7 +3324,9 @@
       <c r="C36" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="D36" s="12"/>
+      <c r="D36" s="12" t="s">
+        <v>235</v>
+      </c>
       <c r="E36" s="12" t="s">
         <v>23</v>
       </c>
@@ -3136,27 +3342,27 @@
       <c r="K36" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="L36" s="45"/>
-      <c r="M36" s="41">
-        <v>1</v>
-      </c>
-      <c r="N36" s="40">
+      <c r="L36" s="44"/>
+      <c r="M36" s="40">
+        <v>1</v>
+      </c>
+      <c r="N36" s="39">
         <v>0</v>
       </c>
-      <c r="O36" s="40">
-        <v>2</v>
-      </c>
-      <c r="P36" s="40">
+      <c r="O36" s="39">
+        <v>2</v>
+      </c>
+      <c r="P36" s="39">
         <v>1</v>
       </c>
       <c r="Q36" s="27">
-        <f>AVERAGE(M36:P36)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R36" s="25"/>
     </row>
-    <row r="37" spans="1:18" ht="42" x14ac:dyDescent="0.15">
-      <c r="A37" s="32">
+    <row r="37" spans="1:18" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A37" s="31">
         <v>33</v>
       </c>
       <c r="B37" s="12" t="s">
@@ -3165,7 +3371,9 @@
       <c r="C37" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D37" s="12"/>
+      <c r="D37" s="12" t="s">
+        <v>236</v>
+      </c>
       <c r="E37" s="12" t="s">
         <v>39</v>
       </c>
@@ -3181,27 +3389,27 @@
       </c>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
-      <c r="L37" s="45"/>
-      <c r="M37" s="41">
-        <v>1</v>
-      </c>
-      <c r="N37" s="40">
-        <v>1</v>
-      </c>
-      <c r="O37" s="40">
-        <v>1</v>
-      </c>
-      <c r="P37" s="40">
+      <c r="L37" s="44"/>
+      <c r="M37" s="40">
+        <v>1</v>
+      </c>
+      <c r="N37" s="39">
+        <v>1</v>
+      </c>
+      <c r="O37" s="39">
+        <v>1</v>
+      </c>
+      <c r="P37" s="39">
         <v>1</v>
       </c>
       <c r="Q37" s="27">
-        <f>AVERAGE(M37:P37)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R37" s="25"/>
     </row>
-    <row r="38" spans="1:18" ht="42" x14ac:dyDescent="0.15">
-      <c r="A38" s="32">
+    <row r="38" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A38" s="31">
         <v>34</v>
       </c>
       <c r="B38" s="12" t="s">
@@ -3210,7 +3418,9 @@
       <c r="C38" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="D38" s="12"/>
+      <c r="D38" s="12" t="s">
+        <v>237</v>
+      </c>
       <c r="E38" s="12" t="s">
         <v>172</v>
       </c>
@@ -3225,20 +3435,20 @@
       <c r="J38" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M38" s="41">
+      <c r="M38" s="40">
         <v>0</v>
       </c>
-      <c r="N38" s="40">
+      <c r="N38" s="39">
         <v>0</v>
       </c>
-      <c r="O38" s="40">
+      <c r="O38" s="39">
         <v>0</v>
       </c>
-      <c r="P38" s="40">
+      <c r="P38" s="39">
         <v>0</v>
       </c>
       <c r="Q38" s="27">
-        <f>AVERAGE(M38:P38)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="R38" s="25"/>
@@ -3258,38 +3468,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="31.5" customWidth="1"/>
-    <col min="4" max="4" width="30.33203125" customWidth="1"/>
-    <col min="5" max="5" width="27.33203125" customWidth="1"/>
-    <col min="6" max="6" width="29.33203125" customWidth="1"/>
-    <col min="7" max="7" width="3.33203125" customWidth="1"/>
-    <col min="8" max="8" width="3.83203125" customWidth="1"/>
-    <col min="9" max="9" width="4.1640625" customWidth="1"/>
-    <col min="10" max="12" width="3.6640625" customWidth="1"/>
-    <col min="13" max="13" width="4.33203125" customWidth="1"/>
-    <col min="14" max="14" width="3.6640625" customWidth="1"/>
-    <col min="15" max="15" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="29.28515625" customWidth="1"/>
+    <col min="7" max="7" width="3.28515625" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" customWidth="1"/>
+    <col min="9" max="9" width="4.140625" customWidth="1"/>
+    <col min="10" max="12" width="3.7109375" customWidth="1"/>
+    <col min="13" max="13" width="4.28515625" customWidth="1"/>
+    <col min="14" max="14" width="3.7109375" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="G3" s="2" t="s">
         <v>2</v>
       </c>
@@ -3299,7 +3509,7 @@
       </c>
       <c r="O3" s="30"/>
     </row>
-    <row r="4" spans="1:22" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:22" ht="27.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>0</v>
       </c>
@@ -3346,7 +3556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:22" s="11" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A5" s="12">
         <v>1</v>
       </c>
@@ -3356,7 +3566,9 @@
       <c r="C5" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="12"/>
+      <c r="D5" s="12" t="s">
+        <v>238</v>
+      </c>
       <c r="E5" s="12" t="s">
         <v>131</v>
       </c>
@@ -3371,20 +3583,20 @@
         <v>4</v>
       </c>
       <c r="J5" s="24"/>
-      <c r="K5" s="42">
-        <v>4</v>
-      </c>
-      <c r="L5" s="37">
-        <v>4</v>
-      </c>
-      <c r="M5" s="39">
-        <v>3</v>
-      </c>
-      <c r="N5" s="37">
+      <c r="K5" s="41">
+        <v>4</v>
+      </c>
+      <c r="L5" s="36">
+        <v>4</v>
+      </c>
+      <c r="M5" s="38">
+        <v>3</v>
+      </c>
+      <c r="N5" s="36">
         <v>3</v>
       </c>
       <c r="O5" s="27">
-        <f>AVERAGE(K5:N5)</f>
+        <f t="shared" ref="O5:O15" si="0">AVERAGE(K5:N5)</f>
         <v>3.5</v>
       </c>
       <c r="P5" s="12"/>
@@ -3395,7 +3607,7 @@
       <c r="U5" s="12"/>
       <c r="V5" s="12"/>
     </row>
-    <row r="6" spans="1:22" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:22" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="12">
         <f>SUM(A5,1)</f>
         <v>2</v>
@@ -3406,7 +3618,9 @@
       <c r="C6" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="12"/>
+      <c r="D6" s="12" t="s">
+        <v>239</v>
+      </c>
       <c r="E6" s="12" t="s">
         <v>136</v>
       </c>
@@ -3419,20 +3633,20 @@
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="26"/>
-      <c r="K6" s="41">
-        <v>4</v>
-      </c>
-      <c r="L6" s="32">
-        <v>4</v>
-      </c>
-      <c r="M6" s="40">
-        <v>2</v>
-      </c>
-      <c r="N6" s="32">
+      <c r="K6" s="40">
+        <v>4</v>
+      </c>
+      <c r="L6" s="31">
+        <v>4</v>
+      </c>
+      <c r="M6" s="39">
+        <v>2</v>
+      </c>
+      <c r="N6" s="31">
         <v>3</v>
       </c>
       <c r="O6" s="27">
-        <f>AVERAGE(K6:N6)</f>
+        <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
       <c r="P6" s="12"/>
@@ -3443,7 +3657,7 @@
       <c r="U6" s="12"/>
       <c r="V6" s="12"/>
     </row>
-    <row r="7" spans="1:22" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:22" s="11" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A7" s="12">
         <f>SUM(A6,1)</f>
         <v>3</v>
@@ -3454,31 +3668,33 @@
       <c r="C7" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="D7" s="12"/>
+      <c r="D7" s="12" t="s">
+        <v>240</v>
+      </c>
       <c r="E7" s="12" t="s">
         <v>181</v>
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="36" t="s">
+      <c r="H7" s="35" t="s">
         <v>4</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="7"/>
-      <c r="K7" s="41">
-        <v>3</v>
-      </c>
-      <c r="L7" s="43">
-        <v>3</v>
-      </c>
-      <c r="M7" s="40">
-        <v>4</v>
-      </c>
-      <c r="N7" s="44">
+      <c r="K7" s="40">
+        <v>3</v>
+      </c>
+      <c r="L7" s="42">
+        <v>3</v>
+      </c>
+      <c r="M7" s="39">
+        <v>4</v>
+      </c>
+      <c r="N7" s="43">
         <v>3</v>
       </c>
       <c r="O7" s="27">
-        <f>AVERAGE(K7:N7)</f>
+        <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
       <c r="P7" s="12"/>
@@ -3489,7 +3705,7 @@
       <c r="U7" s="12"/>
       <c r="V7" s="12"/>
     </row>
-    <row r="8" spans="1:22" s="11" customFormat="1" ht="42" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:22" s="11" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="12">
         <f>SUM(A7,1)</f>
         <v>4</v>
@@ -3500,7 +3716,9 @@
       <c r="C8" s="12" t="s">
         <v>123</v>
       </c>
-      <c r="D8" s="12"/>
+      <c r="D8" s="12" t="s">
+        <v>241</v>
+      </c>
       <c r="E8" s="12" t="s">
         <v>124</v>
       </c>
@@ -3513,20 +3731,20 @@
         <v>4</v>
       </c>
       <c r="J8" s="26"/>
-      <c r="K8" s="41">
-        <v>2</v>
-      </c>
-      <c r="L8" s="32">
-        <v>4</v>
-      </c>
-      <c r="M8" s="40">
-        <v>3</v>
-      </c>
-      <c r="N8" s="32">
+      <c r="K8" s="40">
+        <v>2</v>
+      </c>
+      <c r="L8" s="31">
+        <v>4</v>
+      </c>
+      <c r="M8" s="39">
+        <v>3</v>
+      </c>
+      <c r="N8" s="31">
         <v>2</v>
       </c>
       <c r="O8" s="27">
-        <f>AVERAGE(K8:N8)</f>
+        <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
       <c r="P8" s="12"/>
@@ -3537,7 +3755,7 @@
       <c r="U8" s="12"/>
       <c r="V8" s="12"/>
     </row>
-    <row r="9" spans="1:22" s="11" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:22" s="11" customFormat="1" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A9" s="12">
         <f>SUM(A8,1)</f>
         <v>5</v>
@@ -3548,7 +3766,9 @@
       <c r="C9" s="12" t="s">
         <v>201</v>
       </c>
-      <c r="D9" s="12"/>
+      <c r="D9" s="12" t="s">
+        <v>242</v>
+      </c>
       <c r="E9" s="12" t="s">
         <v>183</v>
       </c>
@@ -3559,20 +3779,20 @@
       </c>
       <c r="I9"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="41">
+      <c r="K9" s="40">
         <v>3</v>
       </c>
       <c r="L9" s="5">
         <v>3</v>
       </c>
-      <c r="M9" s="40">
-        <v>3</v>
-      </c>
-      <c r="N9" s="38">
+      <c r="M9" s="39">
+        <v>3</v>
+      </c>
+      <c r="N9" s="37">
         <v>2</v>
       </c>
       <c r="O9" s="27">
-        <f>AVERAGE(K9:N9)</f>
+        <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
       <c r="P9" s="12"/>
@@ -3583,9 +3803,9 @@
       <c r="U9" s="12"/>
       <c r="V9" s="12"/>
     </row>
-    <row r="10" spans="1:22" s="11" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:22" s="11" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A10" s="12">
-        <f t="shared" ref="A10:A13" si="0">SUM(A9,1)</f>
+        <f t="shared" ref="A10:A13" si="1">SUM(A9,1)</f>
         <v>6</v>
       </c>
       <c r="B10" s="12" t="s">
@@ -3594,7 +3814,9 @@
       <c r="C10" s="12" t="s">
         <v>120</v>
       </c>
-      <c r="D10" s="12"/>
+      <c r="D10" s="12" t="s">
+        <v>243</v>
+      </c>
       <c r="E10" s="12" t="s">
         <v>121</v>
       </c>
@@ -3602,25 +3824,25 @@
         <v>24</v>
       </c>
       <c r="G10" s="25"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="45" t="s">
+      <c r="H10" s="44"/>
+      <c r="I10" s="44" t="s">
         <v>4</v>
       </c>
       <c r="J10" s="26"/>
-      <c r="K10" s="41">
-        <v>2</v>
-      </c>
-      <c r="L10" s="47">
-        <v>2</v>
-      </c>
-      <c r="M10" s="46">
-        <v>2</v>
-      </c>
-      <c r="N10" s="47">
+      <c r="K10" s="40">
+        <v>2</v>
+      </c>
+      <c r="L10" s="46">
+        <v>2</v>
+      </c>
+      <c r="M10" s="45">
+        <v>2</v>
+      </c>
+      <c r="N10" s="46">
         <v>4</v>
       </c>
       <c r="O10" s="27">
-        <f>AVERAGE(K10:N10)</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
       <c r="P10" s="12"/>
@@ -3631,9 +3853,9 @@
       <c r="U10" s="12"/>
       <c r="V10" s="12"/>
     </row>
-    <row r="11" spans="1:22" s="11" customFormat="1" ht="98" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:22" s="11" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="B11" s="12" t="s">
@@ -3642,7 +3864,9 @@
       <c r="C11" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="D11" s="12"/>
+      <c r="D11" s="12" t="s">
+        <v>244</v>
+      </c>
       <c r="E11" s="12" t="s">
         <v>129</v>
       </c>
@@ -3655,20 +3879,20 @@
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
       <c r="J11" s="26"/>
-      <c r="K11" s="41">
-        <v>2</v>
-      </c>
-      <c r="L11" s="32">
-        <v>3</v>
-      </c>
-      <c r="M11" s="40">
-        <v>3</v>
-      </c>
-      <c r="N11" s="32">
+      <c r="K11" s="40">
+        <v>2</v>
+      </c>
+      <c r="L11" s="31">
+        <v>3</v>
+      </c>
+      <c r="M11" s="39">
+        <v>3</v>
+      </c>
+      <c r="N11" s="31">
         <v>2</v>
       </c>
       <c r="O11" s="27">
-        <f>AVERAGE(K11:N11)</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
       <c r="P11" s="12"/>
@@ -3679,9 +3903,9 @@
       <c r="U11" s="12"/>
       <c r="V11" s="12"/>
     </row>
-    <row r="12" spans="1:22" s="11" customFormat="1" ht="84" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:22" s="11" customFormat="1" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A12" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -3690,7 +3914,9 @@
       <c r="C12" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="D12" s="12"/>
+      <c r="D12" s="47" t="s">
+        <v>245</v>
+      </c>
       <c r="E12" s="12" t="s">
         <v>140</v>
       </c>
@@ -3703,20 +3929,20 @@
       <c r="J12" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="K12" s="41">
-        <v>2</v>
-      </c>
-      <c r="L12" s="32">
-        <v>1</v>
-      </c>
-      <c r="M12" s="40">
-        <v>2</v>
-      </c>
-      <c r="N12" s="32">
+      <c r="K12" s="40">
+        <v>2</v>
+      </c>
+      <c r="L12" s="31">
+        <v>1</v>
+      </c>
+      <c r="M12" s="39">
+        <v>2</v>
+      </c>
+      <c r="N12" s="31">
         <v>3</v>
       </c>
       <c r="O12" s="27">
-        <f>AVERAGE(K12:N12)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="P12" s="12"/>
@@ -3727,9 +3953,9 @@
       <c r="U12" s="12"/>
       <c r="V12" s="12"/>
     </row>
-    <row r="13" spans="1:22" ht="60" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:22" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="B13" s="12" t="s">
@@ -3738,38 +3964,40 @@
       <c r="C13" s="12" t="s">
         <v>177</v>
       </c>
-      <c r="D13" s="12"/>
+      <c r="D13" s="12" t="s">
+        <v>246</v>
+      </c>
       <c r="E13" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F13" s="35" t="s">
+      <c r="F13" s="34" t="s">
         <v>179</v>
       </c>
       <c r="G13" s="6"/>
-      <c r="H13" s="36" t="s">
+      <c r="H13" s="35" t="s">
         <v>4</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="41">
-        <v>1</v>
-      </c>
-      <c r="L13" s="43">
-        <v>2</v>
-      </c>
-      <c r="M13" s="40">
-        <v>3</v>
-      </c>
-      <c r="N13" s="44">
+      <c r="K13" s="40">
+        <v>1</v>
+      </c>
+      <c r="L13" s="42">
+        <v>2</v>
+      </c>
+      <c r="M13" s="39">
+        <v>3</v>
+      </c>
+      <c r="N13" s="43">
         <v>2</v>
       </c>
       <c r="O13" s="27">
-        <f>AVERAGE(K13:N13)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" ht="84" x14ac:dyDescent="0.15">
-      <c r="A14" s="32">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="31">
         <v>10</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -3778,7 +4006,9 @@
       <c r="C14" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="D14" s="12"/>
+      <c r="D14" s="47" t="s">
+        <v>247</v>
+      </c>
       <c r="E14" s="12" t="s">
         <v>143</v>
       </c>
@@ -3791,25 +4021,25 @@
       <c r="J14" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="K14" s="41">
-        <v>2</v>
-      </c>
-      <c r="L14" s="32">
-        <v>1</v>
-      </c>
-      <c r="M14" s="40">
-        <v>2</v>
-      </c>
-      <c r="N14" s="32">
+      <c r="K14" s="40">
+        <v>2</v>
+      </c>
+      <c r="L14" s="31">
+        <v>1</v>
+      </c>
+      <c r="M14" s="39">
+        <v>2</v>
+      </c>
+      <c r="N14" s="31">
         <v>2</v>
       </c>
       <c r="O14" s="27">
-        <f>AVERAGE(K14:N14)</f>
+        <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="70" x14ac:dyDescent="0.15">
-      <c r="A15" s="32">
+    <row r="15" spans="1:22" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A15" s="31">
         <v>11</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -3818,7 +4048,9 @@
       <c r="C15" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="D15" s="12"/>
+      <c r="D15" s="47" t="s">
+        <v>248</v>
+      </c>
       <c r="E15" s="12" t="s">
         <v>138</v>
       </c>
@@ -3828,27 +4060,27 @@
       <c r="G15" s="25"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
-      <c r="J15" s="45" t="s">
-        <v>4</v>
-      </c>
-      <c r="K15" s="41">
-        <v>1</v>
-      </c>
-      <c r="L15" s="32">
+      <c r="J15" s="44" t="s">
+        <v>4</v>
+      </c>
+      <c r="K15" s="40">
+        <v>1</v>
+      </c>
+      <c r="L15" s="31">
         <v>0</v>
       </c>
-      <c r="M15" s="40">
-        <v>2</v>
-      </c>
-      <c r="N15" s="32">
+      <c r="M15" s="39">
+        <v>2</v>
+      </c>
+      <c r="N15" s="31">
         <v>2</v>
       </c>
       <c r="O15" s="27">
-        <f>AVERAGE(K15:N15)</f>
+        <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A16" s="12"/>
       <c r="B16" s="12"/>
       <c r="C16" s="12"/>

</xml_diff>

<commit_message>
Removed yellow filling in helist.xlsx
</commit_message>
<xml_diff>
--- a/g2-04-he/helist.xlsx
+++ b/g2-04-he/helist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M4ste\OneDrive\Desktop\HCI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Megaport\Desktop\HCI23\HCI\g2-04-he\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003EA061-D52B-4978-83B0-D37F0DB7C17A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE429B3-810F-4FE6-A2E0-CBEF79502241}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" tabRatio="281" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12675" yWindow="480" windowWidth="23265" windowHeight="18450" tabRatio="281" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problems" sheetId="4" r:id="rId1"/>
@@ -1168,18 +1168,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -1287,7 +1281,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1365,27 +1359,17 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1">
@@ -1394,22 +1378,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1755,7 +1730,7 @@
   <dimension ref="A1:V38"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -1782,12 +1757,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="21" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="32" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1883,16 +1858,16 @@
         <v>4</v>
       </c>
       <c r="L5" s="26"/>
-      <c r="M5" s="40">
-        <v>4</v>
-      </c>
-      <c r="N5" s="39">
-        <v>4</v>
-      </c>
-      <c r="O5" s="39">
-        <v>3</v>
-      </c>
-      <c r="P5" s="39">
+      <c r="M5" s="36">
+        <v>4</v>
+      </c>
+      <c r="N5" s="31">
+        <v>4</v>
+      </c>
+      <c r="O5" s="31">
+        <v>3</v>
+      </c>
+      <c r="P5" s="31">
         <v>3</v>
       </c>
       <c r="Q5" s="27">
@@ -1938,16 +1913,16 @@
       <c r="L6" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="M6" s="40">
-        <v>3</v>
-      </c>
-      <c r="N6" s="39">
-        <v>2</v>
-      </c>
-      <c r="O6" s="39">
-        <v>4</v>
-      </c>
-      <c r="P6" s="39">
+      <c r="M6" s="36">
+        <v>3</v>
+      </c>
+      <c r="N6" s="31">
+        <v>2</v>
+      </c>
+      <c r="O6" s="31">
+        <v>4</v>
+      </c>
+      <c r="P6" s="31">
         <v>4</v>
       </c>
       <c r="Q6" s="27">
@@ -1986,16 +1961,16 @@
       <c r="L7" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="M7" s="40">
-        <v>2</v>
-      </c>
-      <c r="N7" s="39">
-        <v>3</v>
-      </c>
-      <c r="O7" s="39">
-        <v>3</v>
-      </c>
-      <c r="P7" s="39">
+      <c r="M7" s="36">
+        <v>2</v>
+      </c>
+      <c r="N7" s="31">
+        <v>3</v>
+      </c>
+      <c r="O7" s="31">
+        <v>3</v>
+      </c>
+      <c r="P7" s="31">
         <v>4</v>
       </c>
       <c r="Q7" s="27">
@@ -2036,16 +2011,16 @@
       <c r="L8" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="M8" s="40">
-        <v>3</v>
-      </c>
-      <c r="N8" s="39">
-        <v>3</v>
-      </c>
-      <c r="O8" s="39">
-        <v>2</v>
-      </c>
-      <c r="P8" s="39">
+      <c r="M8" s="36">
+        <v>3</v>
+      </c>
+      <c r="N8" s="31">
+        <v>3</v>
+      </c>
+      <c r="O8" s="31">
+        <v>2</v>
+      </c>
+      <c r="P8" s="31">
         <v>3</v>
       </c>
       <c r="Q8" s="27">
@@ -2082,16 +2057,16 @@
         <v>4</v>
       </c>
       <c r="L9" s="26"/>
-      <c r="M9" s="40">
-        <v>2</v>
-      </c>
-      <c r="N9" s="39">
-        <v>3</v>
-      </c>
-      <c r="O9" s="39">
-        <v>3</v>
-      </c>
-      <c r="P9" s="39">
+      <c r="M9" s="36">
+        <v>2</v>
+      </c>
+      <c r="N9" s="31">
+        <v>3</v>
+      </c>
+      <c r="O9" s="31">
+        <v>3</v>
+      </c>
+      <c r="P9" s="31">
         <v>3</v>
       </c>
       <c r="Q9" s="27">
@@ -2130,16 +2105,16 @@
       <c r="L10" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="M10" s="40">
-        <v>2</v>
-      </c>
-      <c r="N10" s="39">
-        <v>3</v>
-      </c>
-      <c r="O10" s="39">
-        <v>3</v>
-      </c>
-      <c r="P10" s="39">
+      <c r="M10" s="36">
+        <v>2</v>
+      </c>
+      <c r="N10" s="31">
+        <v>3</v>
+      </c>
+      <c r="O10" s="31">
+        <v>3</v>
+      </c>
+      <c r="P10" s="31">
         <v>2</v>
       </c>
       <c r="Q10" s="27">
@@ -2176,13 +2151,13 @@
       </c>
       <c r="K11" s="12"/>
       <c r="L11" s="26"/>
-      <c r="M11" s="40">
+      <c r="M11" s="36">
         <v>2</v>
       </c>
       <c r="N11" s="31">
         <v>3</v>
       </c>
-      <c r="O11" s="39">
+      <c r="O11" s="31">
         <v>3</v>
       </c>
       <c r="P11" s="31">
@@ -2221,16 +2196,16 @@
         <v>4</v>
       </c>
       <c r="L12" s="13"/>
-      <c r="M12" s="40">
-        <v>2</v>
-      </c>
-      <c r="N12" s="39">
-        <v>2</v>
-      </c>
-      <c r="O12" s="39">
-        <v>2</v>
-      </c>
-      <c r="P12" s="39">
+      <c r="M12" s="36">
+        <v>2</v>
+      </c>
+      <c r="N12" s="31">
+        <v>2</v>
+      </c>
+      <c r="O12" s="31">
+        <v>2</v>
+      </c>
+      <c r="P12" s="31">
         <v>3</v>
       </c>
       <c r="Q12" s="27">
@@ -2266,16 +2241,16 @@
         <v>4</v>
       </c>
       <c r="L13" s="13"/>
-      <c r="M13" s="40">
-        <v>2</v>
-      </c>
-      <c r="N13" s="39">
-        <v>2</v>
-      </c>
-      <c r="O13" s="39">
-        <v>3</v>
-      </c>
-      <c r="P13" s="39">
+      <c r="M13" s="36">
+        <v>2</v>
+      </c>
+      <c r="N13" s="31">
+        <v>2</v>
+      </c>
+      <c r="O13" s="31">
+        <v>3</v>
+      </c>
+      <c r="P13" s="31">
         <v>2</v>
       </c>
       <c r="Q13" s="27">
@@ -2315,16 +2290,16 @@
         <v>4</v>
       </c>
       <c r="L14" s="26"/>
-      <c r="M14" s="40">
-        <v>2</v>
-      </c>
-      <c r="N14" s="39">
-        <v>1</v>
-      </c>
-      <c r="O14" s="39">
-        <v>3</v>
-      </c>
-      <c r="P14" s="39">
+      <c r="M14" s="36">
+        <v>2</v>
+      </c>
+      <c r="N14" s="31">
+        <v>1</v>
+      </c>
+      <c r="O14" s="31">
+        <v>3</v>
+      </c>
+      <c r="P14" s="31">
         <v>2</v>
       </c>
       <c r="Q14" s="27">
@@ -2362,16 +2337,16 @@
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
       <c r="L15" s="26"/>
-      <c r="M15" s="40">
-        <v>3</v>
-      </c>
-      <c r="N15" s="39">
-        <v>2</v>
-      </c>
-      <c r="O15" s="39">
-        <v>1</v>
-      </c>
-      <c r="P15" s="39">
+      <c r="M15" s="36">
+        <v>3</v>
+      </c>
+      <c r="N15" s="31">
+        <v>2</v>
+      </c>
+      <c r="O15" s="31">
+        <v>1</v>
+      </c>
+      <c r="P15" s="31">
         <v>2</v>
       </c>
       <c r="Q15" s="27">
@@ -2409,16 +2384,16 @@
       <c r="L16" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="M16" s="40">
+      <c r="M16" s="36">
         <v>2</v>
       </c>
       <c r="N16" s="31">
         <v>1</v>
       </c>
-      <c r="O16" s="39">
-        <v>3</v>
-      </c>
-      <c r="P16" s="39">
+      <c r="O16" s="31">
+        <v>3</v>
+      </c>
+      <c r="P16" s="31">
         <v>2</v>
       </c>
       <c r="Q16" s="27">
@@ -2457,16 +2432,16 @@
       <c r="L17" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="M17" s="40">
-        <v>2</v>
-      </c>
-      <c r="N17" s="39">
-        <v>2</v>
-      </c>
-      <c r="O17" s="39">
-        <v>2</v>
-      </c>
-      <c r="P17" s="39">
+      <c r="M17" s="36">
+        <v>2</v>
+      </c>
+      <c r="N17" s="31">
+        <v>2</v>
+      </c>
+      <c r="O17" s="31">
+        <v>2</v>
+      </c>
+      <c r="P17" s="31">
         <v>2</v>
       </c>
       <c r="Q17" s="27">
@@ -2505,16 +2480,16 @@
       <c r="L18" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="M18" s="40">
-        <v>1</v>
-      </c>
-      <c r="N18" s="39">
-        <v>3</v>
-      </c>
-      <c r="O18" s="39">
-        <v>2</v>
-      </c>
-      <c r="P18" s="39">
+      <c r="M18" s="36">
+        <v>1</v>
+      </c>
+      <c r="N18" s="31">
+        <v>3</v>
+      </c>
+      <c r="O18" s="31">
+        <v>2</v>
+      </c>
+      <c r="P18" s="31">
         <v>2</v>
       </c>
       <c r="Q18" s="27">
@@ -2550,16 +2525,16 @@
         <v>4</v>
       </c>
       <c r="L19" s="13"/>
-      <c r="M19" s="40">
-        <v>2</v>
-      </c>
-      <c r="N19" s="39">
-        <v>2</v>
-      </c>
-      <c r="O19" s="39">
-        <v>2</v>
-      </c>
-      <c r="P19" s="39">
+      <c r="M19" s="36">
+        <v>2</v>
+      </c>
+      <c r="N19" s="31">
+        <v>2</v>
+      </c>
+      <c r="O19" s="31">
+        <v>2</v>
+      </c>
+      <c r="P19" s="31">
         <v>2</v>
       </c>
       <c r="Q19" s="27">
@@ -2596,16 +2571,16 @@
         <v>4</v>
       </c>
       <c r="L20" s="26"/>
-      <c r="M20" s="40">
-        <v>2</v>
-      </c>
-      <c r="N20" s="39">
-        <v>2</v>
-      </c>
-      <c r="O20" s="39">
-        <v>1</v>
-      </c>
-      <c r="P20" s="39">
+      <c r="M20" s="36">
+        <v>2</v>
+      </c>
+      <c r="N20" s="31">
+        <v>2</v>
+      </c>
+      <c r="O20" s="31">
+        <v>1</v>
+      </c>
+      <c r="P20" s="31">
         <v>2</v>
       </c>
       <c r="Q20" s="27">
@@ -2642,16 +2617,16 @@
         <v>4</v>
       </c>
       <c r="L21" s="26"/>
-      <c r="M21" s="40">
-        <v>4</v>
-      </c>
-      <c r="N21" s="39">
-        <v>1</v>
-      </c>
-      <c r="O21" s="39">
-        <v>1</v>
-      </c>
-      <c r="P21" s="39">
+      <c r="M21" s="36">
+        <v>4</v>
+      </c>
+      <c r="N21" s="31">
+        <v>1</v>
+      </c>
+      <c r="O21" s="31">
+        <v>1</v>
+      </c>
+      <c r="P21" s="31">
         <v>1</v>
       </c>
       <c r="Q21" s="27">
@@ -2690,16 +2665,16 @@
         <v>4</v>
       </c>
       <c r="L22" s="26"/>
-      <c r="M22" s="40">
-        <v>2</v>
-      </c>
-      <c r="N22" s="39">
-        <v>2</v>
-      </c>
-      <c r="O22" s="39">
-        <v>2</v>
-      </c>
-      <c r="P22" s="39">
+      <c r="M22" s="36">
+        <v>2</v>
+      </c>
+      <c r="N22" s="31">
+        <v>2</v>
+      </c>
+      <c r="O22" s="31">
+        <v>2</v>
+      </c>
+      <c r="P22" s="31">
         <v>1</v>
       </c>
       <c r="Q22" s="27">
@@ -2738,16 +2713,16 @@
       <c r="L23" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="M23" s="45">
-        <v>3</v>
-      </c>
-      <c r="N23" s="39">
-        <v>1</v>
-      </c>
-      <c r="O23" s="39">
-        <v>2</v>
-      </c>
-      <c r="P23" s="39">
+      <c r="M23" s="31">
+        <v>3</v>
+      </c>
+      <c r="N23" s="31">
+        <v>1</v>
+      </c>
+      <c r="O23" s="31">
+        <v>2</v>
+      </c>
+      <c r="P23" s="31">
         <v>1</v>
       </c>
       <c r="Q23" s="27">
@@ -2784,16 +2759,16 @@
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
       <c r="L24" s="26"/>
-      <c r="M24" s="40">
-        <v>2</v>
-      </c>
-      <c r="N24" s="39">
-        <v>2</v>
-      </c>
-      <c r="O24" s="39">
-        <v>2</v>
-      </c>
-      <c r="P24" s="39">
+      <c r="M24" s="36">
+        <v>2</v>
+      </c>
+      <c r="N24" s="31">
+        <v>2</v>
+      </c>
+      <c r="O24" s="31">
+        <v>2</v>
+      </c>
+      <c r="P24" s="31">
         <v>1</v>
       </c>
       <c r="Q24" s="27">
@@ -2830,16 +2805,16 @@
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
       <c r="L25" s="26"/>
-      <c r="M25" s="40">
-        <v>2</v>
-      </c>
-      <c r="N25" s="39">
-        <v>2</v>
-      </c>
-      <c r="O25" s="39">
-        <v>2</v>
-      </c>
-      <c r="P25" s="39">
+      <c r="M25" s="36">
+        <v>2</v>
+      </c>
+      <c r="N25" s="31">
+        <v>2</v>
+      </c>
+      <c r="O25" s="31">
+        <v>2</v>
+      </c>
+      <c r="P25" s="31">
         <v>1</v>
       </c>
       <c r="Q25" s="27">
@@ -2876,16 +2851,16 @@
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
       <c r="L26" s="26"/>
-      <c r="M26" s="40">
-        <v>2</v>
-      </c>
-      <c r="N26" s="39">
-        <v>1</v>
-      </c>
-      <c r="O26" s="39">
-        <v>3</v>
-      </c>
-      <c r="P26" s="39">
+      <c r="M26" s="36">
+        <v>2</v>
+      </c>
+      <c r="N26" s="31">
+        <v>1</v>
+      </c>
+      <c r="O26" s="31">
+        <v>3</v>
+      </c>
+      <c r="P26" s="31">
         <v>1</v>
       </c>
       <c r="Q26" s="27">
@@ -2922,16 +2897,16 @@
       <c r="L27" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="M27" s="40">
-        <v>2</v>
-      </c>
-      <c r="N27" s="39">
-        <v>2</v>
-      </c>
-      <c r="O27" s="39">
-        <v>1</v>
-      </c>
-      <c r="P27" s="39">
+      <c r="M27" s="36">
+        <v>2</v>
+      </c>
+      <c r="N27" s="31">
+        <v>2</v>
+      </c>
+      <c r="O27" s="31">
+        <v>1</v>
+      </c>
+      <c r="P27" s="31">
         <v>2</v>
       </c>
       <c r="Q27" s="27">
@@ -2968,13 +2943,13 @@
       </c>
       <c r="K28" s="12"/>
       <c r="L28" s="26"/>
-      <c r="M28" s="40">
+      <c r="M28" s="36">
         <v>2</v>
       </c>
       <c r="N28" s="31">
         <v>2</v>
       </c>
-      <c r="O28" s="39">
+      <c r="O28" s="31">
         <v>2</v>
       </c>
       <c r="P28" s="31">
@@ -3013,16 +2988,16 @@
         <v>4</v>
       </c>
       <c r="L29" s="13"/>
-      <c r="M29" s="40">
-        <v>3</v>
-      </c>
-      <c r="N29" s="39">
-        <v>2</v>
-      </c>
-      <c r="O29" s="39">
-        <v>1</v>
-      </c>
-      <c r="P29" s="39">
+      <c r="M29" s="36">
+        <v>3</v>
+      </c>
+      <c r="N29" s="31">
+        <v>2</v>
+      </c>
+      <c r="O29" s="31">
+        <v>1</v>
+      </c>
+      <c r="P29" s="31">
         <v>1</v>
       </c>
       <c r="Q29" s="27">
@@ -3058,17 +3033,17 @@
       </c>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
-      <c r="L30" s="44"/>
-      <c r="M30" s="40">
-        <v>2</v>
-      </c>
-      <c r="N30" s="39">
-        <v>2</v>
-      </c>
-      <c r="O30" s="39">
-        <v>1</v>
-      </c>
-      <c r="P30" s="39">
+      <c r="L30" s="12"/>
+      <c r="M30" s="36">
+        <v>2</v>
+      </c>
+      <c r="N30" s="31">
+        <v>2</v>
+      </c>
+      <c r="O30" s="31">
+        <v>1</v>
+      </c>
+      <c r="P30" s="31">
         <v>1</v>
       </c>
       <c r="Q30" s="27">
@@ -3105,17 +3080,17 @@
       </c>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
-      <c r="L31" s="44"/>
-      <c r="M31" s="40">
-        <v>2</v>
-      </c>
-      <c r="N31" s="39">
-        <v>2</v>
-      </c>
-      <c r="O31" s="39">
-        <v>1</v>
-      </c>
-      <c r="P31" s="39">
+      <c r="L31" s="12"/>
+      <c r="M31" s="36">
+        <v>2</v>
+      </c>
+      <c r="N31" s="31">
+        <v>2</v>
+      </c>
+      <c r="O31" s="31">
+        <v>1</v>
+      </c>
+      <c r="P31" s="31">
         <v>1</v>
       </c>
       <c r="Q31" s="27">
@@ -3152,19 +3127,19 @@
       <c r="I32" s="28"/>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
-      <c r="L32" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="M32" s="40">
-        <v>1</v>
-      </c>
-      <c r="N32" s="39">
-        <v>1</v>
-      </c>
-      <c r="O32" s="39">
-        <v>3</v>
-      </c>
-      <c r="P32" s="39">
+      <c r="L32" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M32" s="36">
+        <v>1</v>
+      </c>
+      <c r="N32" s="31">
+        <v>1</v>
+      </c>
+      <c r="O32" s="31">
+        <v>3</v>
+      </c>
+      <c r="P32" s="31">
         <v>1</v>
       </c>
       <c r="Q32" s="27">
@@ -3204,13 +3179,13 @@
       </c>
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
-      <c r="M33" s="40">
+      <c r="M33" s="36">
         <v>1</v>
       </c>
       <c r="N33" s="31">
         <v>1</v>
       </c>
-      <c r="O33" s="39">
+      <c r="O33" s="31">
         <v>3</v>
       </c>
       <c r="P33" s="31">
@@ -3250,17 +3225,17 @@
       </c>
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
-      <c r="L34" s="44"/>
-      <c r="M34" s="40">
-        <v>1</v>
-      </c>
-      <c r="N34" s="39">
-        <v>1</v>
-      </c>
-      <c r="O34" s="39">
-        <v>1</v>
-      </c>
-      <c r="P34" s="39">
+      <c r="L34" s="12"/>
+      <c r="M34" s="36">
+        <v>1</v>
+      </c>
+      <c r="N34" s="31">
+        <v>1</v>
+      </c>
+      <c r="O34" s="31">
+        <v>1</v>
+      </c>
+      <c r="P34" s="31">
         <v>2</v>
       </c>
       <c r="Q34" s="27">
@@ -3296,16 +3271,16 @@
       <c r="J35" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M35" s="40">
-        <v>1</v>
-      </c>
-      <c r="N35" s="39">
-        <v>1</v>
-      </c>
-      <c r="O35" s="39">
-        <v>2</v>
-      </c>
-      <c r="P35" s="39">
+      <c r="M35" s="36">
+        <v>1</v>
+      </c>
+      <c r="N35" s="31">
+        <v>1</v>
+      </c>
+      <c r="O35" s="31">
+        <v>2</v>
+      </c>
+      <c r="P35" s="31">
         <v>1</v>
       </c>
       <c r="Q35" s="27">
@@ -3342,17 +3317,17 @@
       <c r="K36" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="L36" s="44"/>
-      <c r="M36" s="40">
-        <v>1</v>
-      </c>
-      <c r="N36" s="39">
+      <c r="L36" s="12"/>
+      <c r="M36" s="36">
+        <v>1</v>
+      </c>
+      <c r="N36" s="31">
         <v>0</v>
       </c>
-      <c r="O36" s="39">
-        <v>2</v>
-      </c>
-      <c r="P36" s="39">
+      <c r="O36" s="31">
+        <v>2</v>
+      </c>
+      <c r="P36" s="31">
         <v>1</v>
       </c>
       <c r="Q36" s="27">
@@ -3389,17 +3364,17 @@
       </c>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
-      <c r="L37" s="44"/>
-      <c r="M37" s="40">
-        <v>1</v>
-      </c>
-      <c r="N37" s="39">
-        <v>1</v>
-      </c>
-      <c r="O37" s="39">
-        <v>1</v>
-      </c>
-      <c r="P37" s="39">
+      <c r="L37" s="12"/>
+      <c r="M37" s="36">
+        <v>1</v>
+      </c>
+      <c r="N37" s="31">
+        <v>1</v>
+      </c>
+      <c r="O37" s="31">
+        <v>1</v>
+      </c>
+      <c r="P37" s="31">
         <v>1</v>
       </c>
       <c r="Q37" s="27">
@@ -3435,16 +3410,16 @@
       <c r="J38" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="M38" s="40">
+      <c r="M38" s="36">
         <v>0</v>
       </c>
-      <c r="N38" s="39">
+      <c r="N38" s="31">
         <v>0</v>
       </c>
-      <c r="O38" s="39">
+      <c r="O38" s="31">
         <v>0</v>
       </c>
-      <c r="P38" s="39">
+      <c r="P38" s="31">
         <v>0</v>
       </c>
       <c r="Q38" s="27">
@@ -3468,8 +3443,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3583,16 +3558,16 @@
         <v>4</v>
       </c>
       <c r="J5" s="24"/>
-      <c r="K5" s="41">
-        <v>4</v>
-      </c>
-      <c r="L5" s="36">
-        <v>4</v>
-      </c>
-      <c r="M5" s="38">
-        <v>3</v>
-      </c>
-      <c r="N5" s="36">
+      <c r="K5" s="37">
+        <v>4</v>
+      </c>
+      <c r="L5" s="35">
+        <v>4</v>
+      </c>
+      <c r="M5" s="35">
+        <v>3</v>
+      </c>
+      <c r="N5" s="35">
         <v>3</v>
       </c>
       <c r="O5" s="27">
@@ -3633,13 +3608,13 @@
       <c r="H6" s="12"/>
       <c r="I6" s="12"/>
       <c r="J6" s="26"/>
-      <c r="K6" s="40">
+      <c r="K6" s="36">
         <v>4</v>
       </c>
       <c r="L6" s="31">
         <v>4</v>
       </c>
-      <c r="M6" s="39">
+      <c r="M6" s="31">
         <v>2</v>
       </c>
       <c r="N6" s="31">
@@ -3676,21 +3651,21 @@
       </c>
       <c r="F7" s="8"/>
       <c r="G7" s="6"/>
-      <c r="H7" s="35" t="s">
+      <c r="H7" s="34" t="s">
         <v>4</v>
       </c>
       <c r="I7" s="5"/>
       <c r="J7" s="7"/>
-      <c r="K7" s="40">
-        <v>3</v>
-      </c>
-      <c r="L7" s="42">
-        <v>3</v>
-      </c>
-      <c r="M7" s="39">
-        <v>4</v>
-      </c>
-      <c r="N7" s="43">
+      <c r="K7" s="36">
+        <v>3</v>
+      </c>
+      <c r="L7" s="38">
+        <v>3</v>
+      </c>
+      <c r="M7" s="31">
+        <v>4</v>
+      </c>
+      <c r="N7" s="39">
         <v>3</v>
       </c>
       <c r="O7" s="27">
@@ -3731,13 +3706,13 @@
         <v>4</v>
       </c>
       <c r="J8" s="26"/>
-      <c r="K8" s="40">
+      <c r="K8" s="36">
         <v>2</v>
       </c>
       <c r="L8" s="31">
         <v>4</v>
       </c>
-      <c r="M8" s="39">
+      <c r="M8" s="31">
         <v>3</v>
       </c>
       <c r="N8" s="31">
@@ -3779,16 +3754,16 @@
       </c>
       <c r="I9"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="40">
+      <c r="K9" s="36">
         <v>3</v>
       </c>
       <c r="L9" s="5">
         <v>3</v>
       </c>
-      <c r="M9" s="39">
-        <v>3</v>
-      </c>
-      <c r="N9" s="37">
+      <c r="M9" s="31">
+        <v>3</v>
+      </c>
+      <c r="N9" s="31">
         <v>2</v>
       </c>
       <c r="O9" s="27">
@@ -3824,21 +3799,21 @@
         <v>24</v>
       </c>
       <c r="G10" s="25"/>
-      <c r="H10" s="44"/>
-      <c r="I10" s="44" t="s">
+      <c r="H10" s="12"/>
+      <c r="I10" s="12" t="s">
         <v>4</v>
       </c>
       <c r="J10" s="26"/>
-      <c r="K10" s="40">
-        <v>2</v>
-      </c>
-      <c r="L10" s="46">
-        <v>2</v>
-      </c>
-      <c r="M10" s="45">
-        <v>2</v>
-      </c>
-      <c r="N10" s="46">
+      <c r="K10" s="36">
+        <v>2</v>
+      </c>
+      <c r="L10" s="31">
+        <v>2</v>
+      </c>
+      <c r="M10" s="31">
+        <v>2</v>
+      </c>
+      <c r="N10" s="31">
         <v>4</v>
       </c>
       <c r="O10" s="27">
@@ -3879,13 +3854,13 @@
       <c r="H11" s="12"/>
       <c r="I11" s="12"/>
       <c r="J11" s="26"/>
-      <c r="K11" s="40">
+      <c r="K11" s="36">
         <v>2</v>
       </c>
       <c r="L11" s="31">
         <v>3</v>
       </c>
-      <c r="M11" s="39">
+      <c r="M11" s="31">
         <v>3</v>
       </c>
       <c r="N11" s="31">
@@ -3914,7 +3889,7 @@
       <c r="C12" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="D12" s="47" t="s">
+      <c r="D12" s="40" t="s">
         <v>245</v>
       </c>
       <c r="E12" s="12" t="s">
@@ -3929,13 +3904,13 @@
       <c r="J12" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="K12" s="40">
+      <c r="K12" s="36">
         <v>2</v>
       </c>
       <c r="L12" s="31">
         <v>1</v>
       </c>
-      <c r="M12" s="39">
+      <c r="M12" s="31">
         <v>2</v>
       </c>
       <c r="N12" s="31">
@@ -3970,25 +3945,25 @@
       <c r="E13" s="12" t="s">
         <v>178</v>
       </c>
-      <c r="F13" s="34" t="s">
+      <c r="F13" s="33" t="s">
         <v>179</v>
       </c>
       <c r="G13" s="6"/>
-      <c r="H13" s="35" t="s">
+      <c r="H13" s="34" t="s">
         <v>4</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="7"/>
-      <c r="K13" s="40">
-        <v>1</v>
-      </c>
-      <c r="L13" s="42">
-        <v>2</v>
-      </c>
-      <c r="M13" s="39">
-        <v>3</v>
-      </c>
-      <c r="N13" s="43">
+      <c r="K13" s="36">
+        <v>1</v>
+      </c>
+      <c r="L13" s="38">
+        <v>2</v>
+      </c>
+      <c r="M13" s="31">
+        <v>3</v>
+      </c>
+      <c r="N13" s="39">
         <v>2</v>
       </c>
       <c r="O13" s="27">
@@ -4006,7 +3981,7 @@
       <c r="C14" s="12" t="s">
         <v>146</v>
       </c>
-      <c r="D14" s="47" t="s">
+      <c r="D14" s="40" t="s">
         <v>247</v>
       </c>
       <c r="E14" s="12" t="s">
@@ -4021,13 +3996,13 @@
       <c r="J14" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="K14" s="40">
+      <c r="K14" s="36">
         <v>2</v>
       </c>
       <c r="L14" s="31">
         <v>1</v>
       </c>
-      <c r="M14" s="39">
+      <c r="M14" s="31">
         <v>2</v>
       </c>
       <c r="N14" s="31">
@@ -4048,7 +4023,7 @@
       <c r="C15" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="D15" s="47" t="s">
+      <c r="D15" s="40" t="s">
         <v>248</v>
       </c>
       <c r="E15" s="12" t="s">
@@ -4060,16 +4035,16 @@
       <c r="G15" s="25"/>
       <c r="H15" s="12"/>
       <c r="I15" s="12"/>
-      <c r="J15" s="44" t="s">
-        <v>4</v>
-      </c>
-      <c r="K15" s="40">
+      <c r="J15" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K15" s="36">
         <v>1</v>
       </c>
       <c r="L15" s="31">
         <v>0</v>
       </c>
-      <c r="M15" s="39">
+      <c r="M15" s="31">
         <v>2</v>
       </c>
       <c r="N15" s="31">

</xml_diff>